<commit_message>
NEW RULE -  Se a Control Date for maior do que a end date da semana em analise, por como In Process e avisar ao utilizador no excel(XXflagXX) pode ser removido no futuro.
</commit_message>
<xml_diff>
--- a/Migrated_Snapshot.xlsx
+++ b/Migrated_Snapshot.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="135">
   <si>
     <t>ID</t>
   </si>
@@ -277,6 +277,9 @@
   </si>
   <si>
     <t>INC44351758</t>
+  </si>
+  <si>
+    <t>In Process XXflagXX</t>
   </si>
   <si>
     <t>PDF Invoices don't appear in VIM Documents</t>
@@ -505,7 +508,7 @@
     <col min="9" max="9" width="14.36328125" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="14.28125" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="10.19921875" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="13.6953125" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" width="16.48828125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="102.40234375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -1319,16 +1322,16 @@
         <v>17</v>
       </c>
       <c r="L26" t="s" s="0">
-        <v>18</v>
+        <v>88</v>
       </c>
       <c r="M26" t="s" s="0">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0"/>
       <c r="B27" t="s" s="0">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C27" s="0"/>
       <c r="D27" t="s" s="0">
@@ -1353,13 +1356,13 @@
         <v>32</v>
       </c>
       <c r="M27" t="s" s="0">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0"/>
       <c r="B28" t="s" s="0">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C28" s="0"/>
       <c r="D28" t="s" s="0">
@@ -1370,7 +1373,7 @@
       </c>
       <c r="F28" s="0"/>
       <c r="G28" t="s" s="0">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H28" s="0"/>
       <c r="I28" t="n" s="2">
@@ -1384,13 +1387,13 @@
         <v>32</v>
       </c>
       <c r="M28" t="s" s="0">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0"/>
       <c r="B29" t="s" s="0">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C29" s="0"/>
       <c r="D29" t="s" s="0">
@@ -1415,13 +1418,13 @@
         <v>18</v>
       </c>
       <c r="M29" t="s" s="0">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0"/>
       <c r="B30" t="s" s="0">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C30" s="0"/>
       <c r="D30" t="s" s="0">
@@ -1446,13 +1449,13 @@
         <v>18</v>
       </c>
       <c r="M30" t="s" s="0">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0"/>
       <c r="B31" t="s" s="0">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C31" s="0"/>
       <c r="D31" t="s" s="0">
@@ -1477,13 +1480,13 @@
         <v>18</v>
       </c>
       <c r="M31" t="s" s="0">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0"/>
       <c r="B32" t="s" s="0">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C32" s="0"/>
       <c r="D32" t="s" s="0">
@@ -1508,13 +1511,13 @@
         <v>18</v>
       </c>
       <c r="M32" t="s" s="0">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0"/>
       <c r="B33" t="s" s="0">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C33" s="0"/>
       <c r="D33" t="s" s="0">
@@ -1525,7 +1528,7 @@
       </c>
       <c r="F33" s="0"/>
       <c r="G33" t="s" s="0">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H33" s="0"/>
       <c r="I33" t="n" s="2">
@@ -1539,13 +1542,13 @@
         <v>32</v>
       </c>
       <c r="M33" t="s" s="0">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0"/>
       <c r="B34" t="s" s="0">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C34" s="0"/>
       <c r="D34" t="s" s="0">
@@ -1570,13 +1573,13 @@
         <v>18</v>
       </c>
       <c r="M34" t="s" s="0">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0"/>
       <c r="B35" t="s" s="0">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C35" s="0"/>
       <c r="D35" t="s" s="0">
@@ -1601,13 +1604,13 @@
         <v>32</v>
       </c>
       <c r="M35" t="s" s="0">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0"/>
       <c r="B36" t="s" s="0">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C36" s="0"/>
       <c r="D36" t="s" s="0">
@@ -1618,7 +1621,7 @@
       </c>
       <c r="F36" s="0"/>
       <c r="G36" t="s" s="0">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H36" s="0"/>
       <c r="I36" t="n" s="2">
@@ -1629,16 +1632,16 @@
         <v>17</v>
       </c>
       <c r="L36" t="s" s="0">
-        <v>18</v>
+        <v>88</v>
       </c>
       <c r="M36" t="s" s="0">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0"/>
       <c r="B37" t="s" s="0">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C37" s="0"/>
       <c r="D37" t="s" s="0">
@@ -1649,7 +1652,7 @@
       </c>
       <c r="F37" s="0"/>
       <c r="G37" t="s" s="0">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H37" s="0"/>
       <c r="I37" t="n" s="2">
@@ -1663,13 +1666,13 @@
         <v>32</v>
       </c>
       <c r="M37" t="s" s="0">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0"/>
       <c r="B38" t="s" s="0">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C38" s="0"/>
       <c r="D38" t="s" s="0">
@@ -1694,13 +1697,13 @@
         <v>32</v>
       </c>
       <c r="M38" t="s" s="0">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0"/>
       <c r="B39" t="s" s="0">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C39" s="0"/>
       <c r="D39" t="s" s="0">
@@ -1725,13 +1728,13 @@
         <v>32</v>
       </c>
       <c r="M39" t="s" s="0">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0"/>
       <c r="B40" t="s" s="0">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C40" s="0"/>
       <c r="D40" t="s" s="0">
@@ -1756,13 +1759,13 @@
         <v>32</v>
       </c>
       <c r="M40" t="s" s="0">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0"/>
       <c r="B41" t="s" s="0">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C41" s="0"/>
       <c r="D41" t="s" s="0">
@@ -1787,13 +1790,13 @@
         <v>32</v>
       </c>
       <c r="M41" t="s" s="0">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0"/>
       <c r="B42" t="s" s="0">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C42" s="0"/>
       <c r="D42" t="s" s="0">
@@ -1804,7 +1807,7 @@
       </c>
       <c r="F42" s="0"/>
       <c r="G42" t="s" s="0">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H42" s="0"/>
       <c r="I42" t="n" s="2">
@@ -1818,13 +1821,13 @@
         <v>32</v>
       </c>
       <c r="M42" t="s" s="0">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0"/>
       <c r="B43" t="s" s="0">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C43" s="0"/>
       <c r="D43" t="s" s="0">
@@ -1835,7 +1838,7 @@
       </c>
       <c r="F43" s="0"/>
       <c r="G43" t="s" s="0">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H43" s="0"/>
       <c r="I43" t="n" s="2">
@@ -1846,16 +1849,16 @@
         <v>28</v>
       </c>
       <c r="L43" t="s" s="0">
-        <v>18</v>
+        <v>88</v>
       </c>
       <c r="M43" t="s" s="0">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0"/>
       <c r="B44" t="s" s="0">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C44" s="0"/>
       <c r="D44" t="s" s="0">
@@ -1877,10 +1880,10 @@
         <v>28</v>
       </c>
       <c r="L44" t="s" s="0">
-        <v>18</v>
+        <v>88</v>
       </c>
       <c r="M44" t="s" s="0">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1907,7 +1910,7 @@
     <col min="9" max="9" width="14.36328125" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="14.28125" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="10.19921875" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="13.6953125" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" width="16.48828125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="71.3515625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -1955,7 +1958,7 @@
     <row r="2">
       <c r="A2" s="0"/>
       <c r="B2" t="s" s="0">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C2" s="0"/>
       <c r="D2" t="s" s="0">
@@ -1966,7 +1969,7 @@
       </c>
       <c r="F2" s="0"/>
       <c r="G2" t="s" s="0">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H2" s="0"/>
       <c r="I2" t="n" s="4">
@@ -1977,10 +1980,10 @@
         <v>17</v>
       </c>
       <c r="L2" t="s" s="0">
-        <v>18</v>
+        <v>88</v>
       </c>
       <c r="M2" t="s" s="0">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>